<commit_message>
good model find. After this , I do CL
</commit_message>
<xml_diff>
--- a/controllers/CL_TEST_8_action 5/data/Curriculum No ob train 5000_2/Curriculum No ob train 5000_2_Test_heterogeineous_pipe_1/Curriculum No ob train 5000_2_Test_heterogeineous_pipe_1_Test_Result.xlsx
+++ b/controllers/CL_TEST_8_action 5/data/Curriculum No ob train 5000_2/Curriculum No ob train 5000_2_Test_heterogeineous_pipe_1/Curriculum No ob train 5000_2_Test_heterogeineous_pipe_1_Test_Result.xlsx
@@ -448,13 +448,13 @@
         <v>400</v>
       </c>
       <c r="B2" t="n">
-        <v>346</v>
+        <v>399</v>
       </c>
       <c r="C2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D2" t="n">
         <v>0</v>
-      </c>
-      <c r="D2" t="n">
-        <v>54</v>
       </c>
     </row>
     <row r="4">
@@ -476,13 +476,13 @@
     </row>
     <row r="5">
       <c r="B5" t="n">
-        <v>0.865</v>
+        <v>0.9975000000000001</v>
       </c>
       <c r="C5" t="n">
+        <v>0.0025</v>
+      </c>
+      <c r="D5" t="n">
         <v>0</v>
-      </c>
-      <c r="D5" t="n">
-        <v>0.135</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
episode 100 -> GOOD
</commit_message>
<xml_diff>
--- a/controllers/CL_TEST_8_action 5/data/Curriculum No ob train 5000_2/Curriculum No ob train 5000_2_Test_heterogeineous_pipe_1/Curriculum No ob train 5000_2_Test_heterogeineous_pipe_1_Test_Result.xlsx
+++ b/controllers/CL_TEST_8_action 5/data/Curriculum No ob train 5000_2/Curriculum No ob train 5000_2_Test_heterogeineous_pipe_1/Curriculum No ob train 5000_2_Test_heterogeineous_pipe_1_Test_Result.xlsx
@@ -445,13 +445,13 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>400</v>
+        <v>18</v>
       </c>
       <c r="B2" t="n">
-        <v>399</v>
+        <v>18</v>
       </c>
       <c r="C2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D2" t="n">
         <v>0</v>
@@ -476,10 +476,10 @@
     </row>
     <row r="5">
       <c r="B5" t="n">
-        <v>0.9975000000000001</v>
+        <v>1</v>
       </c>
       <c r="C5" t="n">
-        <v>0.0025</v>
+        <v>0</v>
       </c>
       <c r="D5" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
debug memory & model test 애매함. little better.
</commit_message>
<xml_diff>
--- a/controllers/CL_TEST_8_action 5/data/Curriculum No ob train 5000_2/Curriculum No ob train 5000_2_Test_heterogeineous_pipe_1/Curriculum No ob train 5000_2_Test_heterogeineous_pipe_1_Test_Result.xlsx
+++ b/controllers/CL_TEST_8_action 5/data/Curriculum No ob train 5000_2/Curriculum No ob train 5000_2_Test_heterogeineous_pipe_1/Curriculum No ob train 5000_2_Test_heterogeineous_pipe_1_Test_Result.xlsx
@@ -445,13 +445,13 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>18</v>
+        <v>400</v>
       </c>
       <c r="B2" t="n">
-        <v>18</v>
+        <v>387</v>
       </c>
       <c r="C2" t="n">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="D2" t="n">
         <v>0</v>
@@ -476,10 +476,10 @@
     </row>
     <row r="5">
       <c r="B5" t="n">
-        <v>1</v>
+        <v>0.9675</v>
       </c>
       <c r="C5" t="n">
-        <v>0</v>
+        <v>0.0325</v>
       </c>
       <c r="D5" t="n">
         <v>0</v>

</xml_diff>